<commit_message>
Randomized sector selected based on risk tolerance
</commit_message>
<xml_diff>
--- a/frontend/static/Financial Values.xlsx
+++ b/frontend/static/Financial Values.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jesse\Desktop\Financial-Advisor-Senior-Project\frontend\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31B2C75-94C2-4278-AFE9-68B0763AF213}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFCF6197-BA7C-46F2-B670-5824E3CF3E7A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
   <si>
     <t>Objective</t>
   </si>
@@ -115,15 +115,6 @@
   </si>
   <si>
     <t>pricetoearnings</t>
-  </si>
-  <si>
-    <t>Price to Revenue</t>
-  </si>
-  <si>
-    <t>pricetorevenue</t>
-  </si>
-  <si>
-    <t>desc</t>
   </si>
   <si>
     <t>Free Cash Flow to Firm</t>
@@ -447,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -621,7 +612,7 @@
         <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
@@ -632,16 +623,22 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9">
+        <v>2000000000</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
@@ -649,7 +646,7 @@
         <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -657,62 +654,11 @@
       <c r="D10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="E10" t="s">
         <v>23</v>
       </c>
-      <c r="F11">
-        <v>2000000000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12">
+      <c r="F10">
         <v>-99</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>